<commit_message>
third day of the class
</commit_message>
<xml_diff>
--- a/assignment_result.xlsx
+++ b/assignment_result.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8160"/>
+    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8160"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="85">
   <si>
     <t>Anusha178</t>
   </si>
@@ -212,18 +212,12 @@
     <t>indentation missing and latest code missing</t>
   </si>
   <si>
-    <t>Completed but needs latest code merge</t>
-  </si>
-  <si>
     <t>incomplete</t>
   </si>
   <si>
     <t>Harishth</t>
   </si>
   <si>
-    <t>Partially Complete needs latest code</t>
-  </si>
-  <si>
     <t>sachinmoharil</t>
   </si>
   <si>
@@ -234,6 +228,57 @@
   </si>
   <si>
     <t>complete</t>
+  </si>
+  <si>
+    <t>completed (but not needed this much)</t>
+  </si>
+  <si>
+    <t>bhaskar1987</t>
+  </si>
+  <si>
+    <t>completed but who is "Sushma"?</t>
+  </si>
+  <si>
+    <t>completed but code pushed by Sushma. Indentation is missing</t>
+  </si>
+  <si>
+    <t>Completed (found merge conflict)</t>
+  </si>
+  <si>
+    <t>Completed but html tag is missing</t>
+  </si>
+  <si>
+    <t>completed but indentation is missing</t>
+  </si>
+  <si>
+    <t>irapani</t>
+  </si>
+  <si>
+    <t>jayakrishna440</t>
+  </si>
+  <si>
+    <t>krkkrkkrk</t>
+  </si>
+  <si>
+    <t>completed but pay attention to indentation</t>
+  </si>
+  <si>
+    <t>completed but pay attention to spaces</t>
+  </si>
+  <si>
+    <t>partially completed missing &lt;form&gt;</t>
+  </si>
+  <si>
+    <t>partially completed. &lt;githtml&gt; is not valid</t>
+  </si>
+  <si>
+    <t>ravibashetty</t>
+  </si>
+  <si>
+    <t>reddy2006</t>
+  </si>
+  <si>
+    <t>saikaran4423</t>
   </si>
 </sst>
 </file>
@@ -551,16 +596,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AE32"/>
+  <dimension ref="A1:AE39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18.5703125" customWidth="1"/>
     <col min="2" max="2" width="40.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="57.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="34.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:31" x14ac:dyDescent="0.25">
@@ -663,7 +710,10 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>63</v>
+        <v>65</v>
+      </c>
+      <c r="C2" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="3" spans="1:31" x14ac:dyDescent="0.25">
@@ -673,13 +723,19 @@
       <c r="B3" t="s">
         <v>61</v>
       </c>
+      <c r="C3" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="4" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>33</v>
       </c>
       <c r="B4" t="s">
-        <v>63</v>
+        <v>62</v>
+      </c>
+      <c r="C4" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="5" spans="1:31" x14ac:dyDescent="0.25">
@@ -689,221 +745,382 @@
       <c r="B5" t="s">
         <v>61</v>
       </c>
+      <c r="C5" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="6" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>35</v>
+        <v>69</v>
       </c>
       <c r="B6" t="s">
-        <v>63</v>
+        <v>70</v>
+      </c>
+      <c r="C6" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="7" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B7" t="s">
-        <v>63</v>
+        <v>62</v>
+      </c>
+      <c r="C7" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="8" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B8" t="s">
-        <v>63</v>
+        <v>62</v>
+      </c>
+      <c r="C8" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="9" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B9" t="s">
+        <v>62</v>
+      </c>
+      <c r="C9" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="10" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>64</v>
+        <v>38</v>
       </c>
       <c r="B10" t="s">
-        <v>63</v>
+        <v>60</v>
+      </c>
+      <c r="C10" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="11" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>39</v>
+        <v>63</v>
       </c>
       <c r="B11" t="s">
         <v>60</v>
       </c>
+      <c r="C11" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="12" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B12" t="s">
-        <v>62</v>
+        <v>72</v>
+      </c>
+      <c r="C12" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="13" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B13" t="s">
-        <v>63</v>
+        <v>73</v>
+      </c>
+      <c r="C13" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="14" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>42</v>
+        <v>75</v>
       </c>
       <c r="B14" t="s">
-        <v>63</v>
+        <v>62</v>
+      </c>
+      <c r="C14" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="15" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>43</v>
+        <v>77</v>
       </c>
       <c r="B15" t="s">
-        <v>63</v>
+        <v>62</v>
+      </c>
+      <c r="C15" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="16" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
+        <v>76</v>
+      </c>
+      <c r="B16" t="s">
+        <v>62</v>
+      </c>
+      <c r="C16" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>41</v>
+      </c>
+      <c r="B17" t="s">
+        <v>65</v>
+      </c>
+      <c r="C17" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>42</v>
+      </c>
+      <c r="B18" t="s">
+        <v>62</v>
+      </c>
+      <c r="C18" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>43</v>
+      </c>
+      <c r="B19" t="s">
+        <v>62</v>
+      </c>
+      <c r="C19" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
         <v>44</v>
       </c>
-      <c r="B16" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+      <c r="B20" t="s">
+        <v>65</v>
+      </c>
+      <c r="C20" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
         <v>45</v>
       </c>
-      <c r="B17" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+      <c r="B21" t="s">
+        <v>79</v>
+      </c>
+      <c r="C21" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
         <v>46</v>
       </c>
-      <c r="B18" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+      <c r="B22" t="s">
+        <v>65</v>
+      </c>
+      <c r="C22" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
         <v>47</v>
       </c>
-      <c r="B19" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+      <c r="B23" t="s">
+        <v>81</v>
+      </c>
+      <c r="C23" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
         <v>48</v>
       </c>
-      <c r="B20" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
+      <c r="B24" t="s">
+        <v>65</v>
+      </c>
+      <c r="C24" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
         <v>49</v>
       </c>
-      <c r="B21" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
+      <c r="B25" t="s">
+        <v>62</v>
+      </c>
+      <c r="C25" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
         <v>50</v>
       </c>
-      <c r="B22" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
+      <c r="B26" t="s">
+        <v>65</v>
+      </c>
+      <c r="C26" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>82</v>
+      </c>
+      <c r="B27" t="s">
+        <v>62</v>
+      </c>
+      <c r="C27" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>83</v>
+      </c>
+      <c r="B28" t="s">
+        <v>62</v>
+      </c>
+      <c r="C28" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>64</v>
+      </c>
+      <c r="B29" t="s">
+        <v>62</v>
+      </c>
+      <c r="C29" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>84</v>
+      </c>
+      <c r="B30" t="s">
+        <v>62</v>
+      </c>
+      <c r="C30" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>51</v>
+      </c>
+      <c r="B31" t="s">
+        <v>65</v>
+      </c>
+      <c r="C31" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>52</v>
+      </c>
+      <c r="B32" t="s">
+        <v>62</v>
+      </c>
+      <c r="C32" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>53</v>
+      </c>
+      <c r="B33" t="s">
         <v>66</v>
       </c>
-      <c r="B23" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>51</v>
-      </c>
-      <c r="B24" t="s">
+      <c r="C33" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>54</v>
+      </c>
+      <c r="B34" t="s">
+        <v>65</v>
+      </c>
+      <c r="C34" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>55</v>
+      </c>
+      <c r="B35" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>52</v>
-      </c>
-      <c r="B25" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>53</v>
-      </c>
-      <c r="B26" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>54</v>
-      </c>
-      <c r="B27" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>55</v>
-      </c>
-      <c r="B28" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
+      <c r="C35" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
         <v>56</v>
       </c>
-      <c r="B29" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
+      <c r="B36" t="s">
+        <v>62</v>
+      </c>
+      <c r="C36" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
         <v>57</v>
       </c>
-      <c r="B30" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
+      <c r="B37" t="s">
+        <v>62</v>
+      </c>
+      <c r="C37" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
         <v>58</v>
       </c>
-      <c r="B31" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
+      <c r="B38" t="s">
+        <v>62</v>
+      </c>
+      <c r="C38" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
         <v>59</v>
       </c>
-      <c r="B32" t="s">
-        <v>63</v>
+      <c r="B39" t="s">
+        <v>65</v>
+      </c>
+      <c r="C39" t="s">
+        <v>74</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
class on css position
</commit_message>
<xml_diff>
--- a/assignment_result.xlsx
+++ b/assignment_result.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="286" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="318" uniqueCount="114">
   <si>
     <t>Anusha178</t>
   </si>
@@ -334,6 +334,39 @@
   </si>
   <si>
     <t>border of form is missing but everything else is good</t>
+  </si>
+  <si>
+    <t>pay attention to indentation but completed</t>
+  </si>
+  <si>
+    <t>form name cannot have spaces, where is unordered list, style for form is incorrect, where is style for div?</t>
+  </si>
+  <si>
+    <t>FOCUS ON INDENTATION, you were not allowed to use class names hence incomplete</t>
+  </si>
+  <si>
+    <t>perfect</t>
+  </si>
+  <si>
+    <t>indentation is messed up, style for unordered list is incorrect</t>
+  </si>
+  <si>
+    <t>indentation is messed up, good on styles</t>
+  </si>
+  <si>
+    <t>Lsaikumar</t>
+  </si>
+  <si>
+    <t>pay attention to indentation and its list-style: none</t>
+  </si>
+  <si>
+    <t>pay attention to indentation and its &lt;html lang="en"&gt;</t>
+  </si>
+  <si>
+    <t>pay attention to indentation</t>
+  </si>
+  <si>
+    <t>Shirisha9r</t>
   </si>
 </sst>
 </file>
@@ -349,7 +382,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -368,6 +401,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -381,11 +420,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1329,11 +1369,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AE41"/>
+  <dimension ref="A1:AE43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="C1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="C43" sqref="C43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1446,6 +1486,9 @@
       <c r="B2" t="s">
         <v>64</v>
       </c>
+      <c r="C2" t="s">
+        <v>103</v>
+      </c>
     </row>
     <row r="3" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -1454,12 +1497,15 @@
       <c r="B3" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="4" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="C3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="4" spans="1:31" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="3" t="s">
         <v>61</v>
       </c>
     </row>
@@ -1475,6 +1521,9 @@
       <c r="B6" t="s">
         <v>73</v>
       </c>
+      <c r="C6" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="7" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
@@ -1483,6 +1532,9 @@
       <c r="B7" t="s">
         <v>92</v>
       </c>
+      <c r="C7" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="8" spans="1:31" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
@@ -1499,6 +1551,9 @@
       <c r="B9" t="s">
         <v>93</v>
       </c>
+      <c r="C9" s="2" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="10" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
@@ -1507,6 +1562,9 @@
       <c r="B10" t="s">
         <v>64</v>
       </c>
+      <c r="C10" s="2" t="s">
+        <v>104</v>
+      </c>
     </row>
     <row r="11" spans="1:31" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
@@ -1515,6 +1573,9 @@
       <c r="B11" s="2" t="s">
         <v>94</v>
       </c>
+      <c r="C11" s="2" t="s">
+        <v>105</v>
+      </c>
     </row>
     <row r="12" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
@@ -1523,6 +1584,9 @@
       <c r="B12" t="s">
         <v>64</v>
       </c>
+      <c r="C12" s="2" t="s">
+        <v>106</v>
+      </c>
     </row>
     <row r="13" spans="1:31" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
@@ -1531,6 +1595,9 @@
       <c r="B13" s="2" t="s">
         <v>95</v>
       </c>
+      <c r="C13" s="2" t="s">
+        <v>107</v>
+      </c>
     </row>
     <row r="14" spans="1:31" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
@@ -1544,6 +1611,9 @@
       <c r="B15" s="2" t="s">
         <v>96</v>
       </c>
+      <c r="C15" s="2" t="s">
+        <v>108</v>
+      </c>
     </row>
     <row r="16" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
@@ -1552,181 +1622,252 @@
       <c r="B16" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="2" t="s">
+      <c r="C16" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>109</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B17" s="2" t="s">
+      <c r="B18" s="1" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="3" t="s">
+      <c r="C18" s="1" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="3" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="19" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="2" t="s">
+    <row r="20" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="B19" s="2" t="s">
+      <c r="B20" s="1" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="3" t="s">
+      <c r="C20" s="1" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="3" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="21" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="2" t="s">
+    <row r="22" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="B21" s="2" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
+      <c r="B22" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
         <v>89</v>
       </c>
-      <c r="B22" s="2" t="s">
+      <c r="B23" s="2" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
+      <c r="C23" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
         <v>45</v>
       </c>
-      <c r="B23" s="2" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
+      <c r="B24" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="C24" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
         <v>46</v>
       </c>
-      <c r="B24" s="2" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="2" t="s">
+      <c r="B25" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="C25" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="B25" s="2" t="s">
+      <c r="B26" s="4" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="26" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="2" t="s">
+      <c r="C26" s="4" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="B26" s="2" t="s">
+      <c r="B27" s="2" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="27" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="2" t="s">
+      <c r="C27" s="2" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="B27" s="2" t="s">
+      <c r="B28" s="2" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
+      <c r="C28" s="2" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
         <v>80</v>
       </c>
-      <c r="B28" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="2" t="s">
+      <c r="B29" t="s">
+        <v>61</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="B29" s="2" t="s">
+      <c r="B30" s="2" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="30" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="3" t="s">
+      <c r="C30" s="2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="3" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="31" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="3" t="s">
+    <row r="32" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="3" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="32" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="2" t="s">
+    <row r="33" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="B32" s="2" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
+      <c r="B33" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
         <v>50</v>
       </c>
-      <c r="B33" s="2" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
+      <c r="B34" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>113</v>
+      </c>
+      <c r="B35" s="2"/>
+      <c r="C35" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
         <v>51</v>
       </c>
-      <c r="B34" s="2" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="3" t="s">
+      <c r="B36" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="3" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
         <v>53</v>
       </c>
-      <c r="B36" s="2" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
+      <c r="B38" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
         <v>54</v>
       </c>
-      <c r="B37" s="2" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="3" t="s">
+      <c r="B39" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="3" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="39" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="3" t="s">
+    <row r="41" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="3" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="40" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="3" t="s">
+    <row r="42" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="3" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
         <v>58</v>
       </c>
-      <c r="B41" t="s">
+      <c r="B43" t="s">
         <v>77</v>
+      </c>
+      <c r="C43" t="s">
+        <v>61</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
completing the homework from 10/20
</commit_message>
<xml_diff>
--- a/assignment_result.xlsx
+++ b/assignment_result.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="318" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="343" uniqueCount="116">
   <si>
     <t>Anusha178</t>
   </si>
@@ -367,6 +367,12 @@
   </si>
   <si>
     <t>Shirisha9r</t>
+  </si>
+  <si>
+    <t>somushanker01</t>
+  </si>
+  <si>
+    <t>wow! Completed</t>
   </si>
 </sst>
 </file>
@@ -382,7 +388,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -403,7 +409,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF00B0F0"/>
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -420,12 +432,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1369,18 +1382,18 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AE43"/>
+  <dimension ref="A1:AE44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="C43" sqref="C43"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="D1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="21.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="124.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="57.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="96.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="51.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1479,25 +1492,28 @@
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="2" spans="1:31" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B2" t="s">
-        <v>64</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="B2" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="C2" s="4" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="3" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="3" spans="1:31" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="B3" t="s">
-        <v>61</v>
-      </c>
-      <c r="C3" t="s">
+      <c r="B3" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="D3" s="3" t="s">
         <v>61</v>
       </c>
     </row>
@@ -1524,6 +1540,9 @@
       <c r="C6" t="s">
         <v>64</v>
       </c>
+      <c r="D6" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="7" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
@@ -1535,6 +1554,9 @@
       <c r="C7" t="s">
         <v>61</v>
       </c>
+      <c r="D7" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="8" spans="1:31" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
@@ -1543,15 +1565,18 @@
       <c r="B8" s="3" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="9" spans="1:31" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
+      <c r="D8" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="9" spans="1:31" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="C9" s="3" t="s">
         <v>61</v>
       </c>
     </row>
@@ -1565,6 +1590,9 @@
       <c r="C10" s="2" t="s">
         <v>104</v>
       </c>
+      <c r="D10" s="2" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="11" spans="1:31" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
@@ -1576,6 +1604,9 @@
       <c r="C11" s="2" t="s">
         <v>105</v>
       </c>
+      <c r="D11" s="2" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="12" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
@@ -1587,6 +1618,9 @@
       <c r="C12" s="2" t="s">
         <v>106</v>
       </c>
+      <c r="D12" s="2" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="13" spans="1:31" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
@@ -1598,6 +1632,9 @@
       <c r="C13" s="2" t="s">
         <v>107</v>
       </c>
+      <c r="D13" s="2" t="s">
+        <v>115</v>
+      </c>
     </row>
     <row r="14" spans="1:31" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
@@ -1614,59 +1651,74 @@
       <c r="C15" s="2" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="16" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+      <c r="D15" s="2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="16" spans="1:31" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="B16" t="s">
-        <v>61</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+      <c r="B16" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="C17" s="2" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
+      <c r="C17" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="B18" s="5" t="s">
         <v>95</v>
       </c>
-      <c r="C18" s="1" t="s">
+      <c r="C18" s="5" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D18" s="5" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="20" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="1" t="s">
+    <row r="20" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="B20" s="1" t="s">
+      <c r="B20" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="C20" s="1" t="s">
+      <c r="C20" s="5" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D20" s="5" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="22" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
         <v>44</v>
       </c>
@@ -1677,7 +1729,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>89</v>
       </c>
@@ -1687,8 +1739,11 @@
       <c r="C23" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D23" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>45</v>
       </c>
@@ -1698,19 +1753,22 @@
       <c r="C24" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
+      <c r="D24" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="B25" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="C25" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B25" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
         <v>47</v>
       </c>
@@ -1721,7 +1779,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="27" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>48</v>
       </c>
@@ -1731,19 +1789,22 @@
       <c r="C27" s="2" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="2" t="s">
+      <c r="D27" s="2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="B28" s="2" t="s">
+      <c r="B28" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="C28" s="2" t="s">
+      <c r="C28" s="4" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>80</v>
       </c>
@@ -1753,8 +1814,11 @@
       <c r="C29" s="2" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="30" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D29" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>81</v>
       </c>
@@ -1764,18 +1828,21 @@
       <c r="C30" s="2" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D30" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="32" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="33" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
         <v>101</v>
       </c>
@@ -1785,19 +1852,25 @@
       <c r="C33" s="2" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
+      <c r="D33" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="B34" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="C34" s="2" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B34" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="C34" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="D34" s="5" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>113</v>
       </c>
@@ -1805,8 +1878,11 @@
       <c r="C35" s="2" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D35" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>51</v>
       </c>
@@ -1816,57 +1892,73 @@
       <c r="C36" s="2" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="37" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="3" t="s">
+      <c r="D36" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>114</v>
+      </c>
+      <c r="B37" s="2"/>
+      <c r="C37" s="2"/>
+      <c r="D37" s="2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="3" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
+    <row r="39" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="B38" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="C38" s="2" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
+      <c r="B39" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="C39" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="D39" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="B39" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="C39" s="2" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="3" t="s">
+      <c r="B40" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="C40" s="4" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="3" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="41" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="3" t="s">
+    <row r="42" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="3" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="42" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="3" t="s">
+    <row r="43" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="3" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
+    <row r="44" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="B43" t="s">
+      <c r="B44" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="C43" t="s">
+      <c r="C44" s="3" t="s">
         <v>61</v>
       </c>
     </row>

</xml_diff>